<commit_message>
excel file with model data
</commit_message>
<xml_diff>
--- a/results/modelsdata.xlsx
+++ b/results/modelsdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Universidad\TUM\Subjects\3rd semester\Research Internship\ANN_grids\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{477ADC0B-65B6-4070-A789-6573C3E1492F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0C856A3A-0A20-4215-9FFA-969E97087224}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{64DFEDE0-E796-4F06-BF30-0F6C3AC2D19A}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{64DFEDE0-E796-4F06-BF30-0F6C3AC2D19A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,59 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>n_layers</t>
+  </si>
+  <si>
+    <t>layer_1</t>
+  </si>
+  <si>
+    <t>layer_2</t>
+  </si>
+  <si>
+    <t>layer_3</t>
+  </si>
+  <si>
+    <t>layer_4</t>
+  </si>
+  <si>
+    <t>layer_5</t>
+  </si>
+  <si>
+    <t>layer_6</t>
+  </si>
+  <si>
+    <t>layer_7</t>
+  </si>
+  <si>
+    <t>time_steps</t>
+  </si>
+  <si>
+    <t>loss_function</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>validation_split</t>
+  </si>
+  <si>
+    <t>RMSE_best</t>
+  </si>
+  <si>
+    <t>RMSE_av</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +425,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA562FEC-4B29-40B8-B423-B4D14EC15734}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>